<commit_message>
SUCCESS! Scripts work. Need search refinement next.
</commit_message>
<xml_diff>
--- a/ProjectWorkbook.xlsx
+++ b/ProjectWorkbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchung\Personal\SustainabilityScoring\Sustainability\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchung\Personal\SustainabilityScoring\SustainableLLM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C472C48-0E97-4225-AB1B-AA4812ECDF5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CEDDAE-8439-489A-8C29-7A9012A90F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4DFEFFEE-A5F2-4056-B50B-2E496C5164F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{4DFEFFEE-A5F2-4056-B50B-2E496C5164F3}"/>
   </bookViews>
   <sheets>
     <sheet name="User-System Interaction" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="84">
   <si>
     <t>https://www.codesmith.io/blog/introducing-the-emerging-llm-tech-stack</t>
   </si>
@@ -121,9 +121,6 @@
   </si>
   <si>
     <t>Climate W Kai</t>
-  </si>
-  <si>
-    <t>Investing</t>
   </si>
   <si>
     <t>Start writing code</t>
@@ -258,9 +255,6 @@
     <t>Try to query against upserted vectors, test, learn why some failed.</t>
   </si>
   <si>
-    <t>Pinecone_VectorDV_Query.py</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
@@ -281,12 +275,45 @@
   <si>
     <t>Created Pinecone_VectorDB_Query.py but having SSL issues connecting to Pinecone. Probably have to do this on personal device.</t>
   </si>
+  <si>
+    <t>Published new video. Need to add more humor. It is informative and educational, but feel need more humor.</t>
+  </si>
+  <si>
+    <t>Bought more TSM and AR. Dumped some AAPL.</t>
+  </si>
+  <si>
+    <t>Created new repo.</t>
+  </si>
+  <si>
+    <t>Pinecone_VectorDB_Query.py</t>
+  </si>
+  <si>
+    <t>- No results. This is likely a result on uploaded embeddings created differently than input embeddings from query</t>
+  </si>
+  <si>
+    <t>- Go back and redo embeddings using same transformer model. Make sure dimensions are optimized for Pinecone.</t>
+  </si>
+  <si>
+    <t>- Rewrite code to use similar embedding models</t>
+  </si>
+  <si>
+    <t>- Figure out why searches are turning up strange. Rewatch Pinecone Deeplearning video</t>
+  </si>
+  <si>
+    <t>- SUCCESS! Got code to work, now figure out why searches are weird.</t>
+  </si>
+  <si>
+    <t>Success! Three scripts work.</t>
+  </si>
+  <si>
+    <t>Investing/Decision Making</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,6 +360,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -354,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -383,6 +416,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7453,11 +7488,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB258A4-394B-457F-B105-7251391B510B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AC60" sqref="AC60"/>
+    <sheetView showGridLines="0" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AB24" sqref="AB24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7472,7 +7507,7 @@
       <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7484,122 +7519,122 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" style="12" customWidth="1"/>
-    <col min="2" max="2" width="47.1796875" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="21.26953125" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>57</v>
-      </c>
       <c r="C1" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>60</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
         <v>63</v>
       </c>
-      <c r="C5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" t="s">
-        <v>64</v>
-      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>69</v>
-      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="6"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="6"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="6"/>
       <c r="C14" s="3"/>
@@ -7617,9 +7652,9 @@
       <selection activeCell="W79" sqref="W79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7635,70 +7670,66 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A184A6-9F51-4FB6-BFEB-24A808B744E6}">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B47" sqref="B47"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
-    <col min="2" max="2" width="47.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" customWidth="1"/>
-    <col min="4" max="4" width="47.7265625" customWidth="1"/>
-    <col min="5" max="5" width="47.54296875" customWidth="1"/>
-    <col min="6" max="6" width="43.81640625" customWidth="1"/>
-    <col min="7" max="7" width="33.453125" customWidth="1"/>
-    <col min="8" max="8" width="41.1796875" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="47.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="47.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="49.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="47.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="47.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="43.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="33.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="41.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45460</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>A2+1</f>
         <v>45461</v>
@@ -7706,14 +7737,8 @@
       <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f t="shared" ref="A4:A56" si="0">A3+1</f>
         <v>45462</v>
@@ -7721,20 +7746,17 @@
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>45463</v>
@@ -7742,645 +7764,443 @@
       <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>45464</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>45465</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3" t="s">
-        <v>24</v>
+      <c r="D7" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>45466</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>45467</v>
       </c>
-      <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>45468</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>45469</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>45470</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+        <v>37</v>
+      </c>
     </row>
-    <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>45471</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+        <v>38</v>
+      </c>
     </row>
-    <row r="14" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>45472</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>45473</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+        <v>40</v>
+      </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>45474</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>45475</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>45476</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>45477</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>45478</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>45479</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>45480</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+        <v>44</v>
+      </c>
     </row>
-    <row r="23" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>45481</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3" t="s">
+      <c r="C23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>45482</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="4" t="s">
+      <c r="C24" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F24" s="3"/>
       <c r="G24" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>45483</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
+        <v>50</v>
+      </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>45484</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>45485</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>45486</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>45487</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>45488</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>45489</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>45490</v>
       </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <f t="shared" si="0"/>
         <v>45491</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <f t="shared" si="0"/>
         <v>45492</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <f t="shared" si="0"/>
         <v>45493</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <f t="shared" si="0"/>
         <v>45494</v>
       </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <f t="shared" si="0"/>
         <v>45495</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <f t="shared" si="0"/>
         <v>45496</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <f t="shared" si="0"/>
         <v>45497</v>
       </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <f t="shared" si="0"/>
         <v>45498</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <f t="shared" si="0"/>
         <v>45499</v>
       </c>
-      <c r="G41" t="s">
-        <v>71</v>
-      </c>
-      <c r="H41" t="s">
-        <v>72</v>
+      <c r="C41" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <f t="shared" si="0"/>
         <v>45500</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <f t="shared" si="0"/>
         <v>45501</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <f t="shared" si="0"/>
         <v>45502</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <f t="shared" si="0"/>
         <v>45503</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <f t="shared" si="0"/>
         <v>45504</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <f t="shared" si="0"/>
         <v>45505</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <f t="shared" si="0"/>
         <v>45506</v>
       </c>
-      <c r="G48" t="s">
-        <v>70</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>73</v>
+      <c r="B48" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <f t="shared" si="0"/>
         <v>45507</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <f t="shared" si="0"/>
         <v>45508</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <f t="shared" si="0"/>
         <v>45509</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <f t="shared" si="0"/>
         <v>45510</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <f t="shared" si="0"/>
         <v>45511</v>
       </c>
+      <c r="D53" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <f t="shared" si="0"/>
         <v>45512</v>
       </c>
+      <c r="C54" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <f t="shared" si="0"/>
         <v>45513</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <f t="shared" si="0"/>
         <v>45514</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -8390,19 +8210,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C8EE845-60BA-4732-AA2A-75C0592EC76F}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.26953125" customWidth="1"/>
-    <col min="2" max="2" width="19.81640625" customWidth="1"/>
+    <col min="1" max="1" width="67.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -8410,60 +8230,88 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
-        <v>30</v>
+      <c r="B5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B6" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>44</v>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>42</v>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>54</v>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -8477,7 +8325,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated code for PDF processing
</commit_message>
<xml_diff>
--- a/ProjectWorkbook.xlsx
+++ b/ProjectWorkbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markc\PythonAI\SustainableLLM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C259D0A-C2AC-40E1-B708-C706EE304D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735F3F70-86C7-48FA-ABB2-ED8538BC2862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="755" activeTab="3" xr2:uid="{4DFEFFEE-A5F2-4056-B50B-2E496C5164F3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="755" activeTab="5" xr2:uid="{4DFEFFEE-A5F2-4056-B50B-2E496C5164F3}"/>
   </bookViews>
   <sheets>
     <sheet name="User-System Interaction" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="85">
   <si>
     <t>https://www.codesmith.io/blog/introducing-the-emerging-llm-tech-stack</t>
   </si>
@@ -307,6 +307,9 @@
   </si>
   <si>
     <t>Investing/Decision Making</t>
+  </si>
+  <si>
+    <t>-- Dive into PDF processing. Survey, suggest next steps</t>
   </si>
 </sst>
 </file>
@@ -7648,7 +7651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DAFACD3-283B-465D-8EBE-2396B081C61A}">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="W79" sqref="W79"/>
     </sheetView>
   </sheetViews>
@@ -8210,10 +8213,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C8EE845-60BA-4732-AA2A-75C0592EC76F}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView zoomScale="133" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8311,6 +8314,14 @@
         <v>80</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated KG work progress
</commit_message>
<xml_diff>
--- a/ProjectWorkbook.xlsx
+++ b/ProjectWorkbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchung\Personal\SustainabilityScoring\SustainableLLM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF63DF26-DAF9-480B-A8C3-49E448646951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113B0A70-7952-48B0-BACF-2E92E16E7B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="755" activeTab="3" xr2:uid="{4DFEFFEE-A5F2-4056-B50B-2E496C5164F3}"/>
+    <workbookView xWindow="19510" yWindow="20" windowWidth="18800" windowHeight="20820" tabRatio="755" xr2:uid="{4DFEFFEE-A5F2-4056-B50B-2E496C5164F3}"/>
   </bookViews>
   <sheets>
     <sheet name="User-System Interaction" sheetId="1" r:id="rId1"/>
@@ -4180,15 +4180,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>483393</xdr:colOff>
+      <xdr:colOff>486568</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>94176</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>333374</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>75406</xdr:rowOff>
+      <xdr:colOff>336549</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4203,8 +4203,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4733924" y="6761676"/>
-          <a:ext cx="3493294" cy="3791230"/>
+          <a:off x="4737099" y="6344957"/>
+          <a:ext cx="3493294" cy="4549262"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4316,8 +4316,22 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>- Create vector embeddings with data, then upsert to Pinecone</a:t>
-          </a:r>
+            <a:t>- Create vector embeddings with data, then upsert to Pinecone.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>- Similarity function should be close to loss</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> function of embdding model</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1100"/>
@@ -7541,8 +7555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB258A4-394B-457F-B105-7251391B510B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AC24" sqref="AC24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L65" sqref="L65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7701,7 +7715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DAFACD3-283B-465D-8EBE-2396B081C61A}">
   <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>

</xml_diff>